<commit_message>
Update RunTestSuite and LoginTest
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/Heal_Login.xlsx
+++ b/Automation/src/main/java/framework/test/Heal_Login.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Execute</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>60</t>
-  </si>
-  <si>
-    <t>com.gd.wmc.tests.WMCAccountManagementTest</t>
   </si>
   <si>
     <t>N</t>
@@ -492,7 +489,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -526,24 +523,24 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -618,7 +615,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -631,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2">

</xml_diff>

<commit_message>
tests should extends from testbase
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/Heal_Login.xlsx
+++ b/Automation/src/main/java/framework/test/Heal_Login.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/workspace/heal-qa-automation/Automation/src/main/java/framework/test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="18800" windowHeight="10640"/>
+    <workbookView xWindow="240" yWindow="458" windowWidth="18803" windowHeight="10643" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Execute</t>
   </si>
@@ -63,70 +58,106 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>patient.tests.LoginTest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>screenResolution</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Windows 10</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>latest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1280x960</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://patient.qa.heal.com/login</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>browserName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>environment</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>local</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient.tests.VisitTests</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>bookVisit</t>
+  </si>
+  <si>
     <t>Y</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>patient.tests.LoginTest</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>platform</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>screenResolution</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Windows 10</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>latest</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1280x960</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://patient.qa.heal.com/login</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>browserName</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>environment</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>local</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
+    <t>N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>USERNAME</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACCESS_KEY</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RemoteURL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ondemand.saucelabs.com:443/wd/hub</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>qaheal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>e14bb2d7-155b-4775-8978-9365c5b22012</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -141,13 +172,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -156,17 +187,29 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -200,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -208,10 +251,13 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -513,22 +559,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
     <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
-    <col min="4" max="4" width="41.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" customWidth="1"/>
+    <col min="4" max="4" width="41.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.1328125" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,26 +594,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -579,20 +636,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.9"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="3"/>
+    <col min="3" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -600,52 +657,76 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -664,7 +745,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>